<commit_message>
wide for DHS/MICS update
</commit_message>
<xml_diff>
--- a/wide_pipeline/mics_dictionary_setcode.xlsx
+++ b/wide_pipeline/mics_dictionary_setcode.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ado\personal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D77C66A4-2D9E-4B9A-95A6-072BE8C1C2F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6682824-B595-47D5-9FFF-0D8BE0828E51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="605" firstSheet="5" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="605" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dictionary" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2961" uniqueCount="540">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2974" uniqueCount="545">
   <si>
     <t>original_name</t>
   </si>
@@ -1659,6 +1659,21 @@
   </si>
   <si>
     <t>Father's education (up to 17y)</t>
+  </si>
+  <si>
+    <t>Fiji_2021</t>
+  </si>
+  <si>
+    <t>ed6b2</t>
+  </si>
+  <si>
+    <t>only for lesotho mics6 2018</t>
+  </si>
+  <si>
+    <t>ed6b1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">changing this bc this introduces a mistake in LSO 2018, previously it was renamed: ed6c into ed6b </t>
   </si>
 </sst>
 </file>
@@ -1993,10 +2008,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H67"/>
+  <dimension ref="A1:H69"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H65" sqref="H65"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2318,10 +2333,13 @@
         <v>37</v>
       </c>
       <c r="B18" t="s">
-        <v>38</v>
-      </c>
-      <c r="D18" t="s">
-        <v>38</v>
+        <v>37</v>
+      </c>
+      <c r="F18">
+        <v>1</v>
+      </c>
+      <c r="H18" t="s">
+        <v>544</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
@@ -3019,7 +3037,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>536</v>
       </c>
@@ -3033,7 +3051,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>534</v>
       </c>
@@ -3047,7 +3065,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>535</v>
       </c>
@@ -3059,6 +3077,34 @@
       </c>
       <c r="F67">
         <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>541</v>
+      </c>
+      <c r="B68" t="s">
+        <v>541</v>
+      </c>
+      <c r="F68">
+        <v>1</v>
+      </c>
+      <c r="H68" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>543</v>
+      </c>
+      <c r="B69" t="s">
+        <v>543</v>
+      </c>
+      <c r="F69">
+        <v>1</v>
+      </c>
+      <c r="H69" t="s">
+        <v>542</v>
       </c>
     </row>
   </sheetData>
@@ -5033,10 +5079,10 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
-  <dimension ref="A1:J623"/>
+  <dimension ref="A1:J630"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A252" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B278" sqref="B278:C284"/>
+    <sheetView topLeftCell="A585" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C631" sqref="C631"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -11903,6 +11949,83 @@
         <v>9</v>
       </c>
       <c r="C623" s="3">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="624" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A624" t="s">
+        <v>540</v>
+      </c>
+      <c r="B624">
+        <v>0</v>
+      </c>
+      <c r="C624" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="625" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A625" t="s">
+        <v>540</v>
+      </c>
+      <c r="B625">
+        <v>1</v>
+      </c>
+      <c r="C625" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="626" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A626" t="s">
+        <v>540</v>
+      </c>
+      <c r="B626">
+        <v>2</v>
+      </c>
+      <c r="C626" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="627" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A627" t="s">
+        <v>540</v>
+      </c>
+      <c r="B627">
+        <v>3</v>
+      </c>
+      <c r="C627" s="3">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="628" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A628" t="s">
+        <v>540</v>
+      </c>
+      <c r="B628">
+        <v>4</v>
+      </c>
+      <c r="C628" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="629" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A629" t="s">
+        <v>540</v>
+      </c>
+      <c r="B629">
+        <v>8</v>
+      </c>
+      <c r="C629" s="3">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="630" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A630" t="s">
+        <v>540</v>
+      </c>
+      <c r="B630">
+        <v>9</v>
+      </c>
+      <c r="C630" s="3">
         <v>99</v>
       </c>
     </row>
@@ -27057,7 +27180,7 @@
   <dimension ref="A1:B28"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="R48" sqref="R48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>